<commit_message>
cart method and review page methods
</commit_message>
<xml_diff>
--- a/src/main/resources/dadosUsuarios.xlsx
+++ b/src/main/resources/dadosUsuarios.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>FirstName</t>
   </si>
@@ -26,16 +26,22 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Angelo</t>
+    <t>Product</t>
   </si>
   <si>
-    <t>Rodriguez</t>
+    <t>Sanda</t>
   </si>
   <si>
-    <t>li.hirthe@gmail.com</t>
+    <t>Ortiz</t>
   </si>
   <si>
-    <t>bhtzwsl1ya</t>
+    <t>micah.littel@gmail.com</t>
+  </si>
+  <si>
+    <t>fphw2i5ypwj</t>
+  </si>
+  <si>
+    <t>14.1-inch Laptop</t>
   </si>
 </sst>
 </file>
@@ -80,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -99,19 +105,25 @@
       <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove item from cart
</commit_message>
<xml_diff>
--- a/src/main/resources/dadosUsuarios.xlsx
+++ b/src/main/resources/dadosUsuarios.xlsx
@@ -29,16 +29,16 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Sanda</t>
+    <t>Lavern</t>
   </si>
   <si>
-    <t>Ortiz</t>
+    <t>Wiza</t>
   </si>
   <si>
-    <t>micah.littel@gmail.com</t>
+    <t>erasmo.muller@yahoo.com</t>
   </si>
   <si>
-    <t>fphw2i5ypwj</t>
+    <t>kqmp15ef</t>
   </si>
   <si>
     <t>14.1-inch Laptop</t>

</xml_diff>

<commit_message>
config page for CI
</commit_message>
<xml_diff>
--- a/src/main/resources/dadosUsuarios.xlsx
+++ b/src/main/resources/dadosUsuarios.xlsx
@@ -29,16 +29,16 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Emmett</t>
+    <t>Errol</t>
   </si>
   <si>
-    <t>Pagac</t>
+    <t>Lueilwitz</t>
   </si>
   <si>
-    <t>ryan.lang@gmail.com</t>
+    <t>fatimah.kling@gmail.com</t>
   </si>
   <si>
-    <t>f58fwlrf5c</t>
+    <t>ffy04rn7msl</t>
   </si>
   <si>
     <t>14.1-inch Laptop</t>

</xml_diff>

<commit_message>
search product and time response
</commit_message>
<xml_diff>
--- a/src/main/resources/dadosUsuarios.xlsx
+++ b/src/main/resources/dadosUsuarios.xlsx
@@ -29,19 +29,19 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Kendrick</t>
+    <t>Tyrell</t>
   </si>
   <si>
-    <t>Littel</t>
+    <t>Jones</t>
   </si>
   <si>
-    <t>kareem.walter@yahoo.com</t>
+    <t>rickie.lebsack@gmail.com</t>
   </si>
   <si>
-    <t>lfmtm9jrm</t>
+    <t>1b581zkh</t>
   </si>
   <si>
-    <t>7628 Hamill Road</t>
+    <t>46674 Trantow Grove</t>
   </si>
 </sst>
 </file>

</xml_diff>